<commit_message>
need to fix bug at MBBDS
bug that makes miss solutions
</commit_message>
<xml_diff>
--- a/search algorithms comparison.xlsx
+++ b/search algorithms comparison.xlsx
@@ -194,7 +194,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -397,63 +397,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -542,13 +485,117 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -558,7 +605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -587,9 +634,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -602,16 +646,70 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
@@ -620,61 +718,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -999,7 +1052,7 @@
   <dimension ref="D3:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1022,65 +1075,65 @@
   <sheetData>
     <row r="3" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D4" s="11"/>
-      <c r="E4" s="22" t="s">
+      <c r="D4" s="10"/>
+      <c r="E4" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="16" t="s">
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="K4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="L4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="16" t="s">
+      <c r="M4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="16" t="s">
+      <c r="N4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="16" t="s">
+      <c r="O4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="16" t="s">
+      <c r="P4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="Q4" s="17" t="s">
+      <c r="Q4" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="27"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="23"/>
     </row>
     <row r="6" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="E6" s="34" t="s">
+      <c r="E6" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="36"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="27"/>
       <c r="I6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1110,12 +1163,12 @@
       </c>
     </row>
     <row r="7" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="E7" s="34" t="s">
+      <c r="E7" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="36"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="27"/>
       <c r="I7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1145,12 +1198,12 @@
       </c>
     </row>
     <row r="8" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="E8" s="34" t="s">
+      <c r="E8" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="36"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="27"/>
       <c r="I8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1180,131 +1233,131 @@
       </c>
     </row>
     <row r="9" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E9" s="37" t="s">
+      <c r="E9" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" s="13" t="s">
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="13" t="s">
+      <c r="K9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="L9" s="13" t="s">
+      <c r="L9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="M9" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="N9" s="13" t="s">
+      <c r="M9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="N9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="O9" s="13" t="s">
+      <c r="O9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="P9" s="13" t="s">
+      <c r="P9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="Q9" s="14" t="s">
+      <c r="Q9" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="26"/>
-      <c r="Q10" s="27"/>
-    </row>
-    <row r="11" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="E11" s="15" t="s">
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="23"/>
+    </row>
+    <row r="11" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E11" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="I11" s="31" t="s">
+      <c r="I11" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="32"/>
-      <c r="Q11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="33"/>
+      <c r="O11" s="33"/>
+      <c r="P11" s="33"/>
+      <c r="Q11" s="34"/>
     </row>
     <row r="12" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="E12" s="7">
+      <c r="E12" s="35">
+        <v>1</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="37">
         <v>0</v>
       </c>
-      <c r="F12" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="8">
-        <v>0</v>
-      </c>
-      <c r="I12" s="8">
+      <c r="I12" s="37">
         <v>22</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J12" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="K12" s="8">
+      <c r="K12" s="37">
         <v>12</v>
       </c>
-      <c r="L12" s="8">
+      <c r="L12" s="37">
         <f>9*2+12</f>
         <v>30</v>
       </c>
-      <c r="M12" s="8">
+      <c r="M12" s="37">
         <v>22</v>
       </c>
-      <c r="N12" s="8" t="s">
+      <c r="N12" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="O12" s="8">
+      <c r="O12" s="37">
         <v>12</v>
       </c>
-      <c r="P12" s="8">
+      <c r="P12" s="37">
         <v>530</v>
       </c>
-      <c r="Q12" s="6" t="s">
+      <c r="Q12" s="38" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="13" spans="4:17" x14ac:dyDescent="0.3">
       <c r="E13" s="7">
         <f>E12+1</f>
-        <v>1</v>
-      </c>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
+        <v>2</v>
+      </c>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
       <c r="H13" s="8">
         <v>1</v>
       </c>
@@ -1340,14 +1393,14 @@
     <row r="14" spans="4:17" x14ac:dyDescent="0.3">
       <c r="E14" s="7">
         <f t="shared" ref="E14:E21" si="0">E13+1</f>
-        <v>2</v>
-      </c>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
+        <v>3</v>
+      </c>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
       <c r="H14" s="8">
         <v>2</v>
       </c>
-      <c r="I14" s="21">
+      <c r="I14" s="16">
         <v>229820</v>
       </c>
       <c r="J14" s="8" t="s">
@@ -1379,10 +1432,10 @@
     <row r="15" spans="4:17" x14ac:dyDescent="0.3">
       <c r="E15" s="7">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
+        <v>4</v>
+      </c>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
       <c r="H15" s="8">
         <v>3</v>
       </c>
@@ -1414,152 +1467,134 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="E16" s="7">
+    <row r="16" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E16" s="9">
         <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="40">
         <v>4</v>
       </c>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="8">
-        <v>4</v>
-      </c>
-      <c r="I16" s="8">
+      <c r="I16" s="40">
         <v>16841719</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="J16" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="K16" s="8">
+      <c r="K16" s="40">
         <v>6040440</v>
       </c>
-      <c r="L16" s="8">
+      <c r="L16" s="40">
         <f>8123+2*3534074+3*310998+4*20041+5*884+6*25</f>
         <v>8093999</v>
       </c>
-      <c r="M16" s="8">
+      <c r="M16" s="40">
         <v>46599748</v>
       </c>
-      <c r="N16" s="8" t="s">
+      <c r="N16" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="O16" s="8">
+      <c r="O16" s="40">
         <v>23949702</v>
       </c>
-      <c r="P16" s="8">
+      <c r="P16" s="40">
         <v>452135</v>
       </c>
-      <c r="Q16" s="6" t="s">
+      <c r="Q16" s="41" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="5:17" x14ac:dyDescent="0.3">
-      <c r="E17" s="10">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="6"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
     </row>
     <row r="18" spans="5:17" x14ac:dyDescent="0.3">
-      <c r="E18" s="10">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="6"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
     </row>
     <row r="19" spans="5:17" x14ac:dyDescent="0.3">
-      <c r="E19" s="10">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="6"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
     </row>
     <row r="20" spans="5:17" x14ac:dyDescent="0.3">
-      <c r="E20" s="10">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="6"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
     </row>
     <row r="21" spans="5:17" x14ac:dyDescent="0.3">
-      <c r="E21" s="10">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="6"/>
-    </row>
-    <row r="22" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E22" s="9">
-        <f>E21+1</f>
-        <v>10</v>
-      </c>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="19"/>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="20"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+    </row>
+    <row r="22" spans="5:17" x14ac:dyDescent="0.3">
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
added break for A*+IDA*
if it failed on some percentage so i dont want it to continue to a smaller percentage
</commit_message>
<xml_diff>
--- a/search algorithms comparison.xlsx
+++ b/search algorithms comparison.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="42">
   <si>
     <t>Duplicate Detection</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>MBBDS[k]</t>
+  </si>
+  <si>
+    <t>A*+IDA*</t>
   </si>
 </sst>
 </file>
@@ -194,7 +197,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -337,10 +340,34 @@
         <color indexed="64"/>
       </left>
       <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -351,9 +378,96 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -361,6 +475,17 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -370,38 +495,94 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -412,72 +593,23 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -485,23 +617,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -509,94 +634,10 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -605,7 +646,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -619,9 +660,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -643,91 +681,106 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1049,19 +1102,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:Q22"/>
+  <dimension ref="D3:R22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="8.88671875" style="1"/>
-    <col min="5" max="5" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="8.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="2.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="4.21875" style="1" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="8" style="1" bestFit="1" customWidth="1"/>
@@ -1069,71 +1123,76 @@
     <col min="14" max="14" width="15.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.88671875" style="1"/>
+    <col min="17" max="17" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D4" s="10"/>
-      <c r="E4" s="18" t="s">
+    <row r="3" spans="4:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="4:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D4" s="9"/>
+      <c r="E4" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="14" t="s">
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="14" t="s">
+      <c r="L4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="14" t="s">
+      <c r="M4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="14" t="s">
+      <c r="N4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="14" t="s">
+      <c r="O4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="14" t="s">
+      <c r="P4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="Q4" s="15" t="s">
+      <c r="Q4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="R4" s="14" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="E5" s="21" t="s">
+    <row r="5" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="E5" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="23"/>
-    </row>
-    <row r="6" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="E6" s="25" t="s">
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="44"/>
+      <c r="Q5" s="44"/>
+      <c r="R5" s="45"/>
+    </row>
+    <row r="6" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="E6" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="27"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="35"/>
       <c r="I6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1161,14 +1220,17 @@
       <c r="Q6" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="E7" s="25" t="s">
+      <c r="R6" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="E7" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="27"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="35"/>
       <c r="I7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1196,14 +1258,17 @@
       <c r="Q7" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="E8" s="25" t="s">
+      <c r="R7" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="E8" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="27"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="35"/>
       <c r="I8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1228,386 +1293,399 @@
       <c r="P8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="Q8" s="5" t="s">
+      <c r="Q8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="R8" s="26" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E9" s="28" t="s">
+    <row r="9" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="E9" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" s="12" t="s">
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="L9" s="12" t="s">
+      <c r="L9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="M9" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="N9" s="12" t="s">
+      <c r="M9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="N9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="O9" s="12" t="s">
+      <c r="O9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="P9" s="12" t="s">
+      <c r="P9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="Q9" s="13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="E10" s="21" t="s">
+      <c r="Q9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="R9" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="E10" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="23"/>
-    </row>
-    <row r="11" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E11" s="31" t="s">
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="35"/>
+    </row>
+    <row r="11" spans="4:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E11" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="I11" s="32" t="s">
+      <c r="I11" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="33"/>
-      <c r="O11" s="33"/>
-      <c r="P11" s="33"/>
-      <c r="Q11" s="34"/>
-    </row>
-    <row r="12" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="E12" s="35">
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="41"/>
+      <c r="R11" s="42"/>
+    </row>
+    <row r="12" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="E12" s="19">
         <v>1</v>
       </c>
-      <c r="F12" s="36" t="s">
+      <c r="F12" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="36" t="s">
+      <c r="G12" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="37">
+      <c r="H12" s="20">
         <v>0</v>
       </c>
-      <c r="I12" s="37">
+      <c r="I12" s="20">
         <v>22</v>
       </c>
-      <c r="J12" s="37" t="s">
+      <c r="J12" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="K12" s="37">
+      <c r="K12" s="20">
         <v>12</v>
       </c>
-      <c r="L12" s="37">
+      <c r="L12" s="20">
         <f>9*2+12</f>
         <v>30</v>
       </c>
-      <c r="M12" s="37">
+      <c r="M12" s="20">
         <v>22</v>
       </c>
-      <c r="N12" s="37" t="s">
+      <c r="N12" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="O12" s="37">
+      <c r="O12" s="20">
         <v>12</v>
       </c>
-      <c r="P12" s="37">
+      <c r="P12" s="20">
         <v>530</v>
       </c>
-      <c r="Q12" s="38" t="s">
+      <c r="Q12" s="24"/>
+      <c r="R12" s="21" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="E13" s="7">
+    <row r="13" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="E13" s="6">
         <f>E12+1</f>
         <v>2</v>
       </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="8">
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="7">
         <v>1</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="7">
         <v>4882</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="J13" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13" s="7">
         <v>2725</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L13" s="7">
         <f>4*1+78*3+1603*2+1</f>
         <v>3445</v>
       </c>
-      <c r="M13" s="8">
+      <c r="M13" s="7">
         <v>3879</v>
       </c>
-      <c r="N13" s="8" t="s">
+      <c r="N13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="O13" s="8">
+      <c r="O13" s="7">
         <v>2140</v>
       </c>
-      <c r="P13" s="8">
+      <c r="P13" s="7">
         <v>5197</v>
       </c>
-      <c r="Q13" s="6" t="s">
+      <c r="Q13" s="7"/>
+      <c r="R13" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="E14" s="7">
-        <f t="shared" ref="E14:E21" si="0">E13+1</f>
+    <row r="14" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="E14" s="6">
+        <f t="shared" ref="E14:E16" si="0">E13+1</f>
         <v>3</v>
       </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="8">
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="7">
         <v>2</v>
       </c>
-      <c r="I14" s="16">
+      <c r="I14" s="18">
         <v>229820</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="K14" s="8">
+      <c r="K14" s="7">
         <v>75497</v>
       </c>
-      <c r="L14" s="8">
+      <c r="L14" s="7">
         <f>305+2*73147+3*6657+4*472+5*28</f>
         <v>168598</v>
       </c>
-      <c r="M14" s="8">
+      <c r="M14" s="7">
         <v>154816</v>
       </c>
-      <c r="N14" s="8" t="s">
+      <c r="N14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="O14" s="8">
+      <c r="O14" s="7">
         <v>74160</v>
       </c>
-      <c r="P14" s="8">
+      <c r="P14" s="7">
         <v>91679</v>
       </c>
-      <c r="Q14" s="6" t="s">
+      <c r="Q14" s="7"/>
+      <c r="R14" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="E15" s="7">
+    <row r="15" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="E15" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="8">
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="7">
         <v>3</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="7">
         <v>4774950</v>
       </c>
-      <c r="J15" s="8" t="s">
+      <c r="J15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="K15" s="8">
+      <c r="K15" s="7">
         <v>1666515</v>
       </c>
-      <c r="L15" s="8">
+      <c r="L15" s="7">
         <v>2280104</v>
       </c>
-      <c r="M15" s="8">
+      <c r="M15" s="7">
         <v>3308415</v>
       </c>
-      <c r="N15" s="8" t="s">
+      <c r="N15" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="O15" s="8">
+      <c r="O15" s="7">
         <v>1648361</v>
       </c>
-      <c r="P15" s="8">
+      <c r="P15" s="7">
         <v>314799</v>
       </c>
-      <c r="Q15" s="6" t="s">
+      <c r="Q15" s="7"/>
+      <c r="R15" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E16" s="9">
+    <row r="16" spans="4:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E16" s="8">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="40">
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="22">
         <v>4</v>
       </c>
-      <c r="I16" s="40">
+      <c r="I16" s="22">
         <v>16841719</v>
       </c>
-      <c r="J16" s="40" t="s">
+      <c r="J16" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="K16" s="40">
+      <c r="K16" s="22">
         <v>6040440</v>
       </c>
-      <c r="L16" s="40">
+      <c r="L16" s="22">
         <f>8123+2*3534074+3*310998+4*20041+5*884+6*25</f>
         <v>8093999</v>
       </c>
-      <c r="M16" s="40">
+      <c r="M16" s="22">
         <v>46599748</v>
       </c>
-      <c r="N16" s="40" t="s">
+      <c r="N16" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="O16" s="40">
+      <c r="O16" s="22">
         <v>23949702</v>
       </c>
-      <c r="P16" s="40">
+      <c r="P16" s="22">
         <v>452135</v>
       </c>
-      <c r="Q16" s="41" t="s">
+      <c r="Q16" s="25"/>
+      <c r="R16" s="23" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="5:17" x14ac:dyDescent="0.3">
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
-      <c r="N17" s="16"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="16"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
     </row>
     <row r="18" spans="5:17" x14ac:dyDescent="0.3">
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="16"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
     </row>
     <row r="19" spans="5:17" x14ac:dyDescent="0.3">
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="16"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
     </row>
     <row r="20" spans="5:17" x14ac:dyDescent="0.3">
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
-      <c r="N20" s="16"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="16"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
     </row>
     <row r="21" spans="5:17" x14ac:dyDescent="0.3">
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="16"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
     </row>
     <row r="22" spans="5:17" x14ac:dyDescent="0.3">
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="16"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="16"/>
-      <c r="P22" s="16"/>
-      <c r="Q22" s="16"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E5:Q5"/>
     <mergeCell ref="F12:F16"/>
     <mergeCell ref="G12:G16"/>
-    <mergeCell ref="I11:Q11"/>
     <mergeCell ref="E6:H6"/>
     <mergeCell ref="E7:H7"/>
     <mergeCell ref="E8:H8"/>
     <mergeCell ref="E9:H9"/>
-    <mergeCell ref="E10:Q10"/>
+    <mergeCell ref="E10:R10"/>
+    <mergeCell ref="I11:R11"/>
+    <mergeCell ref="E5:R5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>